<commit_message>
refactor: remove Redis session management from AuthService and related configurations
</commit_message>
<xml_diff>
--- a/Expenses.xlsx
+++ b/Expenses.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Q</t>
   </si>
@@ -50,7 +50,208 @@
     <t>Q1</t>
   </si>
   <si>
-    <t/>
+    <t>01/Jul/24</t>
+  </si>
+  <si>
+    <t>GM2</t>
+  </si>
+  <si>
+    <t>Laboratory Work (GST)</t>
+  </si>
+  <si>
+    <t>Sample A</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>02/Jul/24</t>
+  </si>
+  <si>
+    <t>GM3</t>
+  </si>
+  <si>
+    <t>X-ray Services</t>
+  </si>
+  <si>
+    <t>Sample B</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>03/Jul/24</t>
+  </si>
+  <si>
+    <t>GM4</t>
+  </si>
+  <si>
+    <t>Consultation</t>
+  </si>
+  <si>
+    <t>Follow-up</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>04/Jul/24</t>
+  </si>
+  <si>
+    <t>Surgery Fees</t>
+  </si>
+  <si>
+    <t>Urgent</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>05/Jul/24</t>
+  </si>
+  <si>
+    <t>GM5</t>
+  </si>
+  <si>
+    <t>Routine check</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>06/Jul/24</t>
+  </si>
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>Prescription</t>
+  </si>
+  <si>
+    <t>Q7</t>
+  </si>
+  <si>
+    <t>07/Jul/24</t>
+  </si>
+  <si>
+    <t>GM6</t>
+  </si>
+  <si>
+    <t>Initial visit</t>
+  </si>
+  <si>
+    <t>Q8</t>
+  </si>
+  <si>
+    <t>08/Jul/24</t>
+  </si>
+  <si>
+    <t>Follow-up X-ray</t>
+  </si>
+  <si>
+    <t>Q9</t>
+  </si>
+  <si>
+    <t>09/Jul/24</t>
+  </si>
+  <si>
+    <t>GM7</t>
+  </si>
+  <si>
+    <t>Scheduled</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>10/Jul/24</t>
+  </si>
+  <si>
+    <t>Blood Test</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>11/Jul/24</t>
+  </si>
+  <si>
+    <t>Painkiller</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>12/Jul/24</t>
+  </si>
+  <si>
+    <t>Check-up</t>
+  </si>
+  <si>
+    <t>Q13</t>
+  </si>
+  <si>
+    <t>13/Jul/24</t>
+  </si>
+  <si>
+    <t>Chest X-ray</t>
+  </si>
+  <si>
+    <t>Q14</t>
+  </si>
+  <si>
+    <t>14/Jul/24</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>Q15</t>
+  </si>
+  <si>
+    <t>15/Jul/24</t>
+  </si>
+  <si>
+    <t>Urine Test</t>
+  </si>
+  <si>
+    <t>Q16</t>
+  </si>
+  <si>
+    <t>16/Jul/24</t>
+  </si>
+  <si>
+    <t>Vitamin</t>
+  </si>
+  <si>
+    <t>Q17</t>
+  </si>
+  <si>
+    <t>17/Jul/24</t>
+  </si>
+  <si>
+    <t>Q18</t>
+  </si>
+  <si>
+    <t>18/Jul/24</t>
+  </si>
+  <si>
+    <t>Dental X-ray</t>
+  </si>
+  <si>
+    <t>Q19</t>
+  </si>
+  <si>
+    <t>19/Jul/24</t>
+  </si>
+  <si>
+    <t>Emergency</t>
+  </si>
+  <si>
+    <t>Q20</t>
+  </si>
+  <si>
+    <t>20/Jul/24</t>
   </si>
 </sst>
 </file>
@@ -468,25 +669,576 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3">
+        <v>687.5</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>687.5</v>
+      </c>
+      <c r="H2" s="3">
+        <v>22.5</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5">
+        <v>512</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>500</v>
+      </c>
+      <c r="H3" s="5">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1200</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1150</v>
+      </c>
+      <c r="H4" s="3">
+        <v>50</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3500</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3300</v>
+      </c>
+      <c r="H5" s="5">
+        <v>200</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3">
+        <v>800</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>780</v>
+      </c>
+      <c r="H6" s="3">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="5">
+        <v>250</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>240</v>
+      </c>
+      <c r="H7" s="5">
         <v>10</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="I7" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1500</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1450</v>
+      </c>
+      <c r="H8" s="3">
+        <v>50</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="5">
+        <v>680</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>650</v>
+      </c>
+      <c r="H9" s="5">
+        <v>30</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4200</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4000</v>
+      </c>
+      <c r="H10" s="3">
+        <v>200</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5">
+        <v>900</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>880</v>
+      </c>
+      <c r="H11" s="5">
+        <v>20</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="3">
+        <v>300</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3">
+        <v>290</v>
+      </c>
+      <c r="H12" s="3">
         <v>10</v>
       </c>
-      <c r="E2" s="3">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="I12" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1100</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1050</v>
+      </c>
+      <c r="H13" s="5">
+        <v>50</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="3">
+        <v>700</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <v>680</v>
+      </c>
+      <c r="H14" s="3">
+        <v>20</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5000</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>4800</v>
+      </c>
+      <c r="H15" s="5">
+        <v>200</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3">
+        <v>850</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>830</v>
+      </c>
+      <c r="H16" s="3">
+        <v>20</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="5">
+        <v>450</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>440</v>
+      </c>
+      <c r="H17" s="5">
         <v>10</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1300</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1250</v>
+      </c>
+      <c r="H18" s="3">
+        <v>50</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="5">
+        <v>600</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0</v>
+      </c>
+      <c r="G19" s="5">
+        <v>580</v>
+      </c>
+      <c r="H19" s="5">
+        <v>20</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="3">
+        <v>3700</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3">
+        <v>3500</v>
+      </c>
+      <c r="H20" s="3">
+        <v>200</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="5">
+        <v>780</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>760</v>
+      </c>
+      <c r="H21" s="5">
+        <v>20</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>